<commit_message>
move styles to int
</commit_message>
<xml_diff>
--- a/src/zmockup_compiler_unit_test.w3mi.data.xlsx
+++ b/src/zmockup_compiler_unit_test.w3mi.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\mcompiler-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60827D69-03DF-41C9-8931-C0B3414AFE41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087DA2F4-1EBC-4013-98E8-0CEEC164D8B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3342" yWindow="161" windowWidth="26748" windowHeight="14293" activeTab="2" xr2:uid="{E1E9901D-3772-4DF8-B2B7-33B164E4572D}"/>
+    <workbookView xWindow="3342" yWindow="161" windowWidth="26748" windowHeight="14293" activeTab="3" xr2:uid="{E1E9901D-3772-4DF8-B2B7-33B164E4572D}"/>
   </bookViews>
   <sheets>
     <sheet name="_contents" sheetId="3" r:id="rId1"/>
@@ -125,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,12 +135,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,11 +151,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -544,7 +537,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -563,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFD82B1-48E1-4B34-8FC9-F5A4D871A1A1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -619,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5F7552-2D73-4C80-A45E-EDA9FD988D96}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -646,7 +639,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>43344</v>
       </c>
       <c r="C2">
@@ -660,10 +653,10 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>43345</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>16.37</v>
       </c>
       <c r="D3" t="b">
@@ -680,7 +673,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -706,7 +699,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>43344</v>
       </c>
       <c r="C2">
@@ -720,7 +713,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>43345</v>
       </c>
       <c r="C3">
@@ -766,7 +759,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>43344</v>
       </c>
       <c r="C2">
@@ -780,7 +773,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>43345</v>
       </c>
       <c r="C3">

</xml_diff>